<commit_message>
Updated import test files
</commit_message>
<xml_diff>
--- a/ImportApps/TestFiles/China Merchants Bank招商银行.xlsx
+++ b/ImportApps/TestFiles/China Merchants Bank招商银行.xlsx
@@ -251,10 +251,10 @@
     <t>上海国际贸易有限公司</t>
   </si>
   <si>
-    <t>1217952210901</t>
-  </si>
-  <si>
-    <t>许华</t>
+    <t>华</t>
+  </si>
+  <si>
+    <t>1217952XXX901</t>
   </si>
 </sst>
 </file>
@@ -349,8 +349,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -712,10 +712,15 @@
   <dimension ref="A5:AF15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
+    <col min="6" max="6" width="22.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5" spans="1:32">
       <c r="A5" s="1" t="s">
@@ -754,7 +759,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:32">
@@ -774,7 +779,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:32">

</xml_diff>